<commit_message>
negrita en doc y cambios formulas excel
</commit_message>
<xml_diff>
--- a/excel/Book1.xlsx
+++ b/excel/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RealPython\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RealPython\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C04C5004-B57C-4E2F-B74B-CB06117C1827}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3925691-AA4D-46D9-9ECC-76208E590767}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2352" yWindow="1944" windowWidth="17988" windowHeight="9060" xr2:uid="{CBFB64FD-487F-49A2-9F8A-7D18E4AD6768}"/>
   </bookViews>
@@ -380,17 +380,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26541B5-7D0F-429D-870A-EC4B6E06D846}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <f>2+2</f>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>A2+B2</f>
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
number changed on book1.xls
</commit_message>
<xml_diff>
--- a/excel/Book1.xlsx
+++ b/excel/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RealPython\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Real Python\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3925691-AA4D-46D9-9ECC-76208E590767}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D965C8-B063-406D-A86E-3FBFE287B9CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2352" yWindow="1944" windowWidth="17988" windowHeight="9060" xr2:uid="{CBFB64FD-487F-49A2-9F8A-7D18E4AD6768}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A2:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -393,11 +393,11 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <f>A2+B2</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>